<commit_message>
dodano duza macierz doleglosci miast...
</commit_message>
<xml_diff>
--- a/testowanie.xlsx
+++ b/testowanie.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="36">
   <si>
     <t>liczba populacji</t>
   </si>
@@ -480,7 +480,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -612,10 +612,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:I165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="B169" sqref="B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1640,6 +1640,7 @@
       </c>
     </row>
     <row r="79" spans="1:9" ht="15">
+      <c r="B79" s="3"/>
       <c r="D79" s="4">
         <v>2</v>
       </c>
@@ -1679,7 +1680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="4:9" ht="15">
+    <row r="81" spans="1:9" ht="15">
       <c r="D81" s="4">
         <v>4</v>
       </c>
@@ -1699,7 +1700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="4:9" ht="15">
+    <row r="82" spans="1:9" ht="15">
       <c r="D82" s="4">
         <v>5</v>
       </c>
@@ -1717,6 +1718,1098 @@
       </c>
       <c r="I82">
         <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" t="s">
+        <v>1</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="15">
+      <c r="D89" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+    </row>
+    <row r="90" spans="1:9" ht="15">
+      <c r="D90" s="4">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90">
+        <v>2</v>
+      </c>
+      <c r="H90">
+        <v>3</v>
+      </c>
+      <c r="I90">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="15">
+      <c r="D91" s="4">
+        <v>2</v>
+      </c>
+      <c r="E91">
+        <v>2</v>
+      </c>
+      <c r="F91">
+        <v>3</v>
+      </c>
+      <c r="G91">
+        <v>4</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="15">
+      <c r="D92" s="4">
+        <v>3</v>
+      </c>
+      <c r="E92">
+        <v>4</v>
+      </c>
+      <c r="F92">
+        <v>3</v>
+      </c>
+      <c r="G92">
+        <v>2</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="15">
+      <c r="D93" s="4">
+        <v>4</v>
+      </c>
+      <c r="E93">
+        <v>2</v>
+      </c>
+      <c r="F93">
+        <v>3</v>
+      </c>
+      <c r="G93">
+        <v>4</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="15">
+      <c r="D94" s="4">
+        <v>5</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>4</v>
+      </c>
+      <c r="G94">
+        <v>3</v>
+      </c>
+      <c r="H94">
+        <v>2</v>
+      </c>
+      <c r="I94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C98" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" t="s">
+        <v>1</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="15">
+      <c r="D102" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
+      <c r="H102" s="4"/>
+      <c r="I102" s="4"/>
+    </row>
+    <row r="103" spans="1:9" ht="15">
+      <c r="D103" s="4">
+        <v>1</v>
+      </c>
+      <c r="E103">
+        <v>3</v>
+      </c>
+      <c r="F103">
+        <v>4</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="15">
+      <c r="D104" s="4">
+        <v>2</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="F104">
+        <v>2</v>
+      </c>
+      <c r="G104">
+        <v>3</v>
+      </c>
+      <c r="H104">
+        <v>4</v>
+      </c>
+      <c r="I104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="15">
+      <c r="D105" s="4">
+        <v>3</v>
+      </c>
+      <c r="E105">
+        <v>3</v>
+      </c>
+      <c r="F105">
+        <v>4</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <v>1</v>
+      </c>
+      <c r="I105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="15">
+      <c r="D106" s="4">
+        <v>4</v>
+      </c>
+      <c r="E106">
+        <v>1</v>
+      </c>
+      <c r="F106">
+        <v>2</v>
+      </c>
+      <c r="G106">
+        <v>3</v>
+      </c>
+      <c r="H106">
+        <v>4</v>
+      </c>
+      <c r="I106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="15">
+      <c r="D107" s="4">
+        <v>5</v>
+      </c>
+      <c r="E107">
+        <v>3</v>
+      </c>
+      <c r="F107">
+        <v>2</v>
+      </c>
+      <c r="G107">
+        <v>1</v>
+      </c>
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" t="s">
+        <v>0</v>
+      </c>
+      <c r="B110">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C111" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" t="s">
+        <v>3</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
+      <c r="A113" t="s">
+        <v>1</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="15">
+      <c r="D114" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+      <c r="H114" s="4"/>
+      <c r="I114" s="4"/>
+    </row>
+    <row r="115" spans="1:9" ht="15">
+      <c r="D115" s="4">
+        <v>1</v>
+      </c>
+      <c r="E115">
+        <v>4</v>
+      </c>
+      <c r="F115">
+        <v>3</v>
+      </c>
+      <c r="G115">
+        <v>2</v>
+      </c>
+      <c r="H115">
+        <v>1</v>
+      </c>
+      <c r="I115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="15">
+      <c r="D116" s="4">
+        <v>2</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
+      </c>
+      <c r="F116">
+        <v>2</v>
+      </c>
+      <c r="G116">
+        <v>3</v>
+      </c>
+      <c r="H116">
+        <v>4</v>
+      </c>
+      <c r="I116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="15">
+      <c r="D117" s="4">
+        <v>3</v>
+      </c>
+      <c r="E117">
+        <v>3</v>
+      </c>
+      <c r="F117">
+        <v>4</v>
+      </c>
+      <c r="G117">
+        <v>0</v>
+      </c>
+      <c r="H117">
+        <v>1</v>
+      </c>
+      <c r="I117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="15">
+      <c r="D118" s="4">
+        <v>4</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="F118">
+        <v>0</v>
+      </c>
+      <c r="G118">
+        <v>4</v>
+      </c>
+      <c r="H118">
+        <v>3</v>
+      </c>
+      <c r="I118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="15">
+      <c r="D119" s="4">
+        <v>5</v>
+      </c>
+      <c r="E119">
+        <v>4</v>
+      </c>
+      <c r="F119">
+        <v>3</v>
+      </c>
+      <c r="G119">
+        <v>2</v>
+      </c>
+      <c r="H119">
+        <v>1</v>
+      </c>
+      <c r="I119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="A122" t="s">
+        <v>0</v>
+      </c>
+      <c r="B122">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C123" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
+      <c r="A124" t="s">
+        <v>3</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="A125" t="s">
+        <v>1</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="15">
+      <c r="D126" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="4"/>
+      <c r="H126" s="4"/>
+      <c r="I126" s="4"/>
+    </row>
+    <row r="127" spans="1:9" ht="15">
+      <c r="D127" s="4">
+        <v>1</v>
+      </c>
+      <c r="E127">
+        <v>1</v>
+      </c>
+      <c r="F127">
+        <v>2</v>
+      </c>
+      <c r="G127">
+        <v>3</v>
+      </c>
+      <c r="H127">
+        <v>4</v>
+      </c>
+      <c r="I127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="15">
+      <c r="D128" s="4">
+        <v>2</v>
+      </c>
+      <c r="E128">
+        <v>1</v>
+      </c>
+      <c r="F128">
+        <v>0</v>
+      </c>
+      <c r="G128">
+        <v>4</v>
+      </c>
+      <c r="H128">
+        <v>3</v>
+      </c>
+      <c r="I128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" ht="15">
+      <c r="D129" s="4">
+        <v>3</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+      <c r="F129">
+        <v>2</v>
+      </c>
+      <c r="G129">
+        <v>3</v>
+      </c>
+      <c r="H129">
+        <v>4</v>
+      </c>
+      <c r="I129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="15">
+      <c r="D130" s="4">
+        <v>4</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <v>1</v>
+      </c>
+      <c r="G130">
+        <v>2</v>
+      </c>
+      <c r="H130">
+        <v>3</v>
+      </c>
+      <c r="I130">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="15">
+      <c r="D131" s="4">
+        <v>5</v>
+      </c>
+      <c r="E131">
+        <v>1</v>
+      </c>
+      <c r="F131">
+        <v>2</v>
+      </c>
+      <c r="G131">
+        <v>3</v>
+      </c>
+      <c r="H131">
+        <v>4</v>
+      </c>
+      <c r="I131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="A132" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="A133" t="s">
+        <v>0</v>
+      </c>
+      <c r="B133">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
+      <c r="A134" t="s">
+        <v>2</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C134" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9">
+      <c r="A135" t="s">
+        <v>3</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
+      <c r="A136" t="s">
+        <v>1</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="15">
+      <c r="D137" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E137" s="4"/>
+      <c r="F137" s="4"/>
+      <c r="G137" s="4"/>
+      <c r="H137" s="4"/>
+      <c r="I137" s="4"/>
+    </row>
+    <row r="138" spans="1:9" ht="15">
+      <c r="D138" s="4">
+        <v>1</v>
+      </c>
+      <c r="E138">
+        <v>2</v>
+      </c>
+      <c r="F138">
+        <v>3</v>
+      </c>
+      <c r="G138">
+        <v>4</v>
+      </c>
+      <c r="H138">
+        <v>0</v>
+      </c>
+      <c r="I138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="15">
+      <c r="D139" s="4">
+        <v>2</v>
+      </c>
+      <c r="E139">
+        <v>1</v>
+      </c>
+      <c r="F139">
+        <v>0</v>
+      </c>
+      <c r="G139">
+        <v>4</v>
+      </c>
+      <c r="H139">
+        <v>3</v>
+      </c>
+      <c r="I139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="15">
+      <c r="D140" s="4">
+        <v>3</v>
+      </c>
+      <c r="E140">
+        <v>2</v>
+      </c>
+      <c r="F140">
+        <v>3</v>
+      </c>
+      <c r="G140">
+        <v>4</v>
+      </c>
+      <c r="H140">
+        <v>0</v>
+      </c>
+      <c r="I140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="15">
+      <c r="D141" s="4">
+        <v>4</v>
+      </c>
+      <c r="E141">
+        <v>3</v>
+      </c>
+      <c r="F141">
+        <v>2</v>
+      </c>
+      <c r="G141">
+        <v>1</v>
+      </c>
+      <c r="H141">
+        <v>0</v>
+      </c>
+      <c r="I141">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="15">
+      <c r="D142" s="4">
+        <v>5</v>
+      </c>
+      <c r="E142">
+        <v>4</v>
+      </c>
+      <c r="F142">
+        <v>3</v>
+      </c>
+      <c r="G142">
+        <v>2</v>
+      </c>
+      <c r="H142">
+        <v>1</v>
+      </c>
+      <c r="I142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9">
+      <c r="A143" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9">
+      <c r="A144" t="s">
+        <v>0</v>
+      </c>
+      <c r="B144">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9">
+      <c r="A145" t="s">
+        <v>2</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C145" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9">
+      <c r="A146" t="s">
+        <v>3</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9">
+      <c r="A147" t="s">
+        <v>1</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" ht="15">
+      <c r="D148" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E148" s="4"/>
+      <c r="F148" s="4"/>
+      <c r="G148" s="4"/>
+      <c r="H148" s="4"/>
+      <c r="I148" s="4"/>
+    </row>
+    <row r="149" spans="1:9" ht="15">
+      <c r="D149" s="4">
+        <v>1</v>
+      </c>
+      <c r="E149">
+        <v>1</v>
+      </c>
+      <c r="F149">
+        <v>0</v>
+      </c>
+      <c r="G149">
+        <v>4</v>
+      </c>
+      <c r="H149">
+        <v>3</v>
+      </c>
+      <c r="I149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" ht="15">
+      <c r="D150" s="4">
+        <v>2</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+      <c r="F150">
+        <v>4</v>
+      </c>
+      <c r="G150">
+        <v>3</v>
+      </c>
+      <c r="H150">
+        <v>2</v>
+      </c>
+      <c r="I150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" ht="15">
+      <c r="D151" s="4">
+        <v>3</v>
+      </c>
+      <c r="E151">
+        <v>2</v>
+      </c>
+      <c r="F151">
+        <v>1</v>
+      </c>
+      <c r="G151">
+        <v>0</v>
+      </c>
+      <c r="H151">
+        <v>4</v>
+      </c>
+      <c r="I151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" ht="15">
+      <c r="D152" s="4">
+        <v>4</v>
+      </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
+      <c r="F152">
+        <v>1</v>
+      </c>
+      <c r="G152">
+        <v>2</v>
+      </c>
+      <c r="H152">
+        <v>3</v>
+      </c>
+      <c r="I152">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" ht="15">
+      <c r="D153" s="4">
+        <v>5</v>
+      </c>
+      <c r="E153">
+        <v>1</v>
+      </c>
+      <c r="F153">
+        <v>0</v>
+      </c>
+      <c r="G153">
+        <v>4</v>
+      </c>
+      <c r="H153">
+        <v>3</v>
+      </c>
+      <c r="I153">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9">
+      <c r="A155" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9">
+      <c r="A156" t="s">
+        <v>0</v>
+      </c>
+      <c r="B156">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9">
+      <c r="A157" t="s">
+        <v>2</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9">
+      <c r="A158" t="s">
+        <v>3</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9">
+      <c r="A159" t="s">
+        <v>1</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="15">
+      <c r="D160" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E160" s="4"/>
+      <c r="F160" s="4"/>
+      <c r="G160" s="4"/>
+      <c r="H160" s="4"/>
+      <c r="I160" s="4"/>
+    </row>
+    <row r="161" spans="4:9" ht="15">
+      <c r="D161" s="4">
+        <v>1</v>
+      </c>
+      <c r="E161">
+        <v>0</v>
+      </c>
+      <c r="F161">
+        <v>1</v>
+      </c>
+      <c r="G161">
+        <v>2</v>
+      </c>
+      <c r="H161">
+        <v>3</v>
+      </c>
+      <c r="I161">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="4:9" ht="15">
+      <c r="D162" s="4">
+        <v>2</v>
+      </c>
+      <c r="E162">
+        <v>1</v>
+      </c>
+      <c r="F162">
+        <v>0</v>
+      </c>
+      <c r="G162">
+        <v>4</v>
+      </c>
+      <c r="H162">
+        <v>3</v>
+      </c>
+      <c r="I162">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="4:9" ht="15">
+      <c r="D163" s="4">
+        <v>3</v>
+      </c>
+      <c r="E163">
+        <v>3</v>
+      </c>
+      <c r="F163">
+        <v>4</v>
+      </c>
+      <c r="G163">
+        <v>0</v>
+      </c>
+      <c r="H163">
+        <v>1</v>
+      </c>
+      <c r="I163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="4:9" ht="15">
+      <c r="D164" s="4">
+        <v>4</v>
+      </c>
+      <c r="E164">
+        <v>3</v>
+      </c>
+      <c r="F164">
+        <v>2</v>
+      </c>
+      <c r="G164">
+        <v>1</v>
+      </c>
+      <c r="H164">
+        <v>0</v>
+      </c>
+      <c r="I164">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="4:9" ht="15">
+      <c r="D165" s="4">
+        <v>5</v>
+      </c>
+      <c r="E165">
+        <v>4</v>
+      </c>
+      <c r="F165">
+        <v>3</v>
+      </c>
+      <c r="G165">
+        <v>2</v>
+      </c>
+      <c r="H165">
+        <v>1</v>
+      </c>
+      <c r="I165">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>